<commit_message>
added holders to spreadsheet and other fuctionality
</commit_message>
<xml_diff>
--- a/Sample Folder/MC12 Tool Usage Data.xlsx
+++ b/Sample Folder/MC12 Tool Usage Data.xlsx
@@ -439,6 +439,11 @@
           <t>FACE MILL</t>
         </is>
       </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>C50-10SM2</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -457,6 +462,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>C50F3-10SF394-9</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -475,6 +485,11 @@
           <t>DOVETAIL</t>
         </is>
       </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>C50-50EM4</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -493,6 +508,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -511,6 +531,11 @@
           <t>SPOT</t>
         </is>
       </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER600</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -529,6 +554,11 @@
           <t>DRILL</t>
         </is>
       </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER600</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -547,6 +577,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -565,6 +600,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -583,6 +623,11 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -601,6 +646,11 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -619,6 +669,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -637,6 +692,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER400</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -655,6 +715,11 @@
           <t>FACE MILL</t>
         </is>
       </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>C50-10SM4</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -673,6 +738,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -691,6 +761,11 @@
           <t>SINGLE</t>
         </is>
       </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -709,6 +784,11 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER600</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -727,6 +807,11 @@
           <t>REAMER</t>
         </is>
       </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -745,6 +830,11 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -763,6 +853,11 @@
           <t>BOTTOM</t>
         </is>
       </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -781,6 +876,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>C50-62SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -799,6 +899,11 @@
           <t>SPOT</t>
         </is>
       </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -817,6 +922,11 @@
           <t>BORING BAR BUILD UP</t>
         </is>
       </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -835,6 +945,11 @@
           <t>BORING BAR BUILD UP</t>
         </is>
       </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -853,6 +968,11 @@
           <t>DRILL</t>
         </is>
       </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -871,6 +991,11 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>C50-25SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -889,6 +1014,11 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -907,6 +1037,7 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -925,6 +1056,7 @@
           <t>DRILL</t>
         </is>
       </c>
+      <c r="E29" s="2" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -943,6 +1075,7 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -961,6 +1094,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>C50-25SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -979,6 +1117,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -997,6 +1140,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -1015,6 +1163,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -1033,6 +1186,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -1051,6 +1209,11 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER600</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -1069,6 +1232,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -1087,6 +1255,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -1105,6 +1278,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1123,6 +1301,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -1141,6 +1324,11 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1159,6 +1347,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1177,6 +1370,11 @@
           <t>DOUBLE</t>
         </is>
       </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -1195,6 +1393,11 @@
           <t>BALL NOSE</t>
         </is>
       </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>C50-25SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -1213,6 +1416,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -1231,6 +1439,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF315-9</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -1249,6 +1462,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>C50-50SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -1267,6 +1485,11 @@
           <t>COOLANT THRU</t>
         </is>
       </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>C50-32ER600</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -1285,6 +1508,11 @@
           <t>DRILL</t>
         </is>
       </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -1303,6 +1531,11 @@
           <t>DRILL</t>
         </is>
       </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>C50-16ER400</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -1321,6 +1554,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>C50-25SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -1339,6 +1577,11 @@
           <t>BULL NOSE</t>
         </is>
       </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>C50-38SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -1357,6 +1600,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>C50-25SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -1375,6 +1623,11 @@
           <t>ENDMILL</t>
         </is>
       </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>C50-75SF630-9</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -1391,6 +1644,11 @@
       <c r="D55" s="2" t="inlineStr">
         <is>
           <t>WHEEL CUTTER</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>C50-10EM4</t>
         </is>
       </c>
     </row>
@@ -1509,10 +1767,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>357</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>61.02564102564103</v>
+        <v>48.10126582278481</v>
       </c>
     </row>
     <row r="3">
@@ -1522,10 +1780,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>38.11965811965812</v>
+        <v>50.63291139240506</v>
       </c>
     </row>
     <row r="4">
@@ -1535,10 +1793,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.8547008547008548</v>
+        <v>1.265822784810127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>